<commit_message>
optimization + corrections price calulation
</commit_message>
<xml_diff>
--- a/cartes.xlsx
+++ b/cartes.xlsx
@@ -7,7 +7,7 @@
     <sheet name="CommandesData" sheetId="2" r:id="rId2"/>
     <sheet name="Feuille" sheetId="3" r:id="rId3"/>
     <sheet name="Feuil1" sheetId="4" r:id="rId4"/>
-    <sheet name="10_03_2025" sheetId="5" r:id="rId5"/>
+    <sheet name="11_03_2025" sheetId="5" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
@@ -16480,7 +16480,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Eevee-Heroes/Umbreon-V-V3-s6a085?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G2" s="1">
-        <v>227.98</v>
+        <v>227.62</v>
       </c>
     </row>
     <row r="3">
@@ -16526,7 +16526,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Eevee-Heroes/Sylveon-VMAX-V1-s6a041?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G4" s="1">
-        <v>1.78</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="5">
@@ -16549,7 +16549,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Eevee-Heroes/Umbreon-VMAX-V1?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G5" s="1">
-        <v>3.38</v>
+        <v>3.31</v>
       </c>
     </row>
     <row r="6">
@@ -16618,7 +16618,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Eevee-Heroes/Vaporeon-V-V1?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G8" s="1">
-        <v>0.87</v>
+        <v>0.94</v>
       </c>
     </row>
     <row r="9">
@@ -16664,7 +16664,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Blue-Sky-Stream/Trevenant-V-V2?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G10" s="1">
-        <v>2.03</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11">
@@ -16940,7 +16940,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Galarian-Moltres-V-V1-s8b096?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G22" s="1">
-        <v>0.36</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="23">
@@ -17078,7 +17078,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Flareon-V2-s8b188?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G28" s="1">
-        <v>7.11</v>
+        <v>7.3</v>
       </c>
     </row>
     <row r="29">
@@ -17101,7 +17101,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Eevee-V2-s8b210?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G29" s="1">
-        <v>8</v>
+        <v>7.8</v>
       </c>
     </row>
     <row r="30">
@@ -17147,7 +17147,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Corviknight-V-V2-s8b248?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G31" s="1">
-        <v>4.17</v>
+        <v>4.33</v>
       </c>
     </row>
     <row r="32">
@@ -17170,7 +17170,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Machamp-V-s12a071?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G32" s="1">
-        <v>0.32</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="33">
@@ -17239,7 +17239,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Regigigas-V-s12a124?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G35" s="1">
-        <v>0.08</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="36">
@@ -17262,7 +17262,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Mewtwo-V-s12a050?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G36" s="1">
-        <v>0.43</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="37">
@@ -17308,7 +17308,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Oricorio-V2-s12a176?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G38" s="1">
-        <v>0.77</v>
+        <v>0.63</v>
       </c>
     </row>
     <row r="39">
@@ -17469,7 +17469,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Gardenias-Vigor-V2-s12a243?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G45" s="1">
-        <v>14.58</v>
+        <v>14.38</v>
       </c>
     </row>
     <row r="46">
@@ -17492,7 +17492,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Zacian-V-V2-s12a225?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G46" s="1">
-        <v>10.96</v>
+        <v>10.81</v>
       </c>
     </row>
     <row r="47">
@@ -17515,7 +17515,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Radiant-Charizard-s12a015?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G47" s="1">
-        <v>2.96</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48">
@@ -17538,7 +17538,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Entei-V-V2-s12a213?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G48" s="1">
-        <v>15.96</v>
+        <v>15.81</v>
       </c>
     </row>
     <row r="49">
@@ -17561,7 +17561,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Rayquaza-VMAX-s12a108?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G49" s="1">
-        <v>0.82</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="50">
@@ -17584,7 +17584,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Origin-Forme-Palkia-VSTAR-V1-s12a028?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G50" s="1">
-        <v>0.48</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="51">
@@ -17676,7 +17676,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Miltank-V2-s12a199?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G54" s="1">
-        <v>0.98</v>
+        <v>1.32</v>
       </c>
     </row>
     <row r="55">
@@ -17745,7 +17745,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Giratina-V-s12a110?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G57" s="1">
-        <v>0.38</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="58">
@@ -17837,7 +17837,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Psychic-Energy-s12a255?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G61" s="1">
-        <v>0.13</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="62">
@@ -17860,7 +17860,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Radiant-Hawlucha-s12a078?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G62" s="1">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="63">
@@ -17906,7 +17906,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Giratina-VSTAR-V2-s12a261?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G64" s="1">
-        <v>129.9</v>
+        <v>130.8</v>
       </c>
     </row>
     <row r="65">
@@ -17998,7 +17998,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Regigigas-VSTAR-V2-s12a233?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G68" s="1">
-        <v>7.17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="69">
@@ -18021,7 +18021,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Entei-V-V2-s12a213?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G69" s="1">
-        <v>15.96</v>
+        <v>15.81</v>
       </c>
     </row>
     <row r="70">
@@ -18044,7 +18044,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Suicune-V-V2-s12a215?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G70" s="1">
-        <v>25.15</v>
+        <v>25.16</v>
       </c>
     </row>
     <row r="71">
@@ -18067,7 +18067,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Hisuian-Samurott-V-V2-s12a229?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G71" s="1">
-        <v>6.4</v>
+        <v>6.48</v>
       </c>
     </row>
     <row r="72">
@@ -18090,7 +18090,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Darkrai-VSTAR-s12a228?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G72" s="1">
-        <v>17.16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="73">
@@ -18113,7 +18113,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Deoxys-VMAX-s12a222?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G73" s="1">
-        <v>12.23</v>
+        <v>12.32</v>
       </c>
     </row>
     <row r="74">
@@ -18136,7 +18136,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Zacian-V-V2-s12a225?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G74" s="1">
-        <v>10.96</v>
+        <v>10.81</v>
       </c>
     </row>
     <row r="75">
@@ -18182,7 +18182,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Hisuian-Samurott-VSTAR-V2-s12a230?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G76" s="1">
-        <v>4.66</v>
+        <v>4.13</v>
       </c>
     </row>
     <row r="77">
@@ -18205,7 +18205,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Raikou-V-V2-s12a218?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G77" s="1">
-        <v>17.32</v>
+        <v>17.12</v>
       </c>
     </row>
     <row r="78">
@@ -18251,7 +18251,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Keldeo-V2-s12a179?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G79" s="1">
-        <v>3.18</v>
+        <v>2.71</v>
       </c>
     </row>
     <row r="80">
@@ -18297,7 +18297,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Magmortar-V2-s12a175?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G81" s="1">
-        <v>1.95</v>
+        <v>1.94</v>
       </c>
     </row>
     <row r="82">
@@ -18320,7 +18320,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Lapras-V2-s12a177?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G82" s="1">
-        <v>3</v>
+        <v>3.04</v>
       </c>
     </row>
     <row r="83">
@@ -18412,7 +18412,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Absol-V2-s12a191?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G86" s="1">
-        <v>1.99</v>
+        <v>1.96</v>
       </c>
     </row>
     <row r="87">
@@ -18481,7 +18481,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Hisuian-Voltorb-V2-s12a173?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G89" s="1">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="90">
@@ -18527,7 +18527,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Mew-V2-s12a183?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G91" s="1">
-        <v>14.32</v>
+        <v>14.49</v>
       </c>
     </row>
     <row r="92">
@@ -18596,7 +18596,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Galarian-Moltres-V2-s12a190?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G94" s="1">
-        <v>4.96</v>
+        <v>4.95</v>
       </c>
     </row>
     <row r="95">
@@ -18642,7 +18642,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Galarian-Articuno-V2-s12a182?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G96" s="1">
-        <v>1.41</v>
+        <v>1.46</v>
       </c>
     </row>
     <row r="97">
@@ -18688,7 +18688,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/151/Giovannis-Charisma-V3-MEW204?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=2&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G98" s="1">
-        <v>26.5</v>
+        <v>28.97</v>
       </c>
     </row>
     <row r="99">
@@ -18711,7 +18711,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VSTAR-Universe/Hisuian-Voltorb-V2-s12a173?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G99" s="1">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="100">
@@ -18734,7 +18734,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Clay-Burst/Grafaiai-V2-sv2D080?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G100" s="1">
-        <v>0.87</v>
+        <v>0.83</v>
       </c>
     </row>
     <row r="101">
@@ -18803,7 +18803,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Castform-V2-s8b211?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G103" s="1">
-        <v>0.46</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="104">
@@ -18895,7 +18895,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Scarlet-ex/Sandile-V2-sv1S087?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G107" s="1">
-        <v>1.26</v>
+        <v>1.22</v>
       </c>
     </row>
     <row r="108">
@@ -18941,7 +18941,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Dark-Phantasma/Hisuian-Arcanine-V2-s10a075?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G109" s="1">
-        <v>1.27</v>
+        <v>1.13</v>
       </c>
     </row>
     <row r="110">
@@ -18987,7 +18987,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Scarlet-ex/Klawf-V2-sv1S088?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G111" s="1">
-        <v>0.93</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="112">
@@ -19010,7 +19010,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Ariados-V2-s8b205?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G112" s="1">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="113">
@@ -19056,7 +19056,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Battle-Region/Wyrdeer-V2-s9a070?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G114" s="1">
-        <v>0.47</v>
+        <v>0.57</v>
       </c>
     </row>
     <row r="115">
@@ -19102,7 +19102,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Battle-Region/Hoothoot-V2-s9a073?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G116" s="1">
-        <v>1.17</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="117">
@@ -19125,7 +19125,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Incandescent-Arcana/Smeargle-V2-s11a073?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G117" s="1">
-        <v>1</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="118">
@@ -19148,7 +19148,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Snow-Hazard/Orthworm-V2-sv2P081?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G118" s="1">
-        <v>0.93</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="119">
@@ -19171,7 +19171,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Alcremie-V2-s8b201?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G119" s="1">
-        <v>0.81</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="120">
@@ -19194,7 +19194,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Shiny-Treasure-ex/Charizard-ex-V1-sv4a115?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G120" s="1">
-        <v>0.42</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="121">
@@ -19355,7 +19355,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Shiny-Treasure-ex/Pidgeot-ex-V1-sv4a139?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G127" s="1">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="128">
@@ -19470,7 +19470,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Shiny-Treasure-ex/Iron-Treads-ex-V1-sv4a132?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G132" s="1">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="133">
@@ -19493,7 +19493,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Shiny-Treasure-ex/Glimmora-ex-V1-sv4a111?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G133" s="1">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="134">
@@ -19746,7 +19746,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Dawn-Dash/Gardevoir-Lv55-DP4d?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G144" s="1">
-        <v>9.91</v>
+        <v>9.9</v>
       </c>
     </row>
     <row r="145">
@@ -19769,7 +19769,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Dawn-Dash/Sceptile-Lv52-DP4d?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=3&amp;isReverseHolo=N</v>
       </c>
       <c r="G145" s="1">
-        <v>4.27</v>
+        <v>3.78</v>
       </c>
     </row>
     <row r="146">
@@ -19815,7 +19815,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Emerald-Break/Shaymin-EX-V1-XY6063?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G147" s="1">
-        <v>7.5</v>
+        <v>6.48</v>
       </c>
     </row>
     <row r="148">
@@ -19884,7 +19884,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/GX-Ultra-Shiny/Reshiram-GX-sm8b018?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G150" s="1">
-        <v>1.95</v>
+        <v>1.85</v>
       </c>
     </row>
     <row r="151">
@@ -20114,7 +20114,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Frosmoth-V2-s8b192?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G160" s="1">
-        <v>1</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="161">
@@ -20137,7 +20137,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Kingdra-V2-s8b190?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G161" s="1">
-        <v>3.02</v>
+        <v>2.86</v>
       </c>
     </row>
     <row r="162">
@@ -20252,7 +20252,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Incandescent-Arcana/Alolan-Vulpix-VSTAR-V1-s11a023?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G166" s="1">
-        <v>0.52</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="167">
@@ -20321,7 +20321,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Incandescent-Arcana/Milotic-V2-s11a070?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G169" s="1">
-        <v>3.68</v>
+        <v>3.49</v>
       </c>
     </row>
     <row r="170">
@@ -20344,7 +20344,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Incandescent-Arcana/Gardevoir-V2-s11a072?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G170" s="1">
-        <v>2.93</v>
+        <v>2.86</v>
       </c>
     </row>
     <row r="171">
@@ -20367,7 +20367,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Ruler-of-the-Black-Flame/Gloom-V2-sv3109?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G171" s="1">
-        <v>3.85</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="172">
@@ -20390,7 +20390,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Ruler-of-the-Black-Flame/Ninetales-V2-sv3110?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G172" s="1">
-        <v>7.93</v>
+        <v>7.83</v>
       </c>
     </row>
     <row r="173">
@@ -20413,7 +20413,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Ruler-of-the-Black-Flame/Scizor-V2-sv3116?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G173" s="1">
-        <v>3.75</v>
+        <v>3.93</v>
       </c>
     </row>
     <row r="174">
@@ -20505,7 +20505,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/VMAX-Climax/Zekrom-V2-s8b195?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G177" s="1">
-        <v>16.9</v>
+        <v>16.99</v>
       </c>
     </row>
     <row r="178">
@@ -20620,7 +20620,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Shiny-Collection/Cinccino?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G182" s="1">
-        <v>10.67</v>
+        <v>9.19</v>
       </c>
     </row>
     <row r="183">
@@ -20689,7 +20689,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Shiny-Collection/Torchic?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G185" s="1">
-        <v>4.15</v>
+        <v>3.39</v>
       </c>
     </row>
     <row r="186">
@@ -20735,7 +20735,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Shiny-Collection/Teddiursa?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G187" s="1">
-        <v>3.99</v>
+        <v>3.47</v>
       </c>
     </row>
     <row r="188">
@@ -20781,7 +20781,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Shiny-Collection/Minccino?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G189" s="1">
-        <v>3.11</v>
+        <v>2.65</v>
       </c>
     </row>
     <row r="190">
@@ -20873,7 +20873,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Secret-of-the-Lakes/Azelf-Lv50-DP2?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=3&amp;isReverseHolo=N</v>
       </c>
       <c r="G193" s="1">
-        <v>6</v>
+        <v>6.48</v>
       </c>
     </row>
     <row r="194">
@@ -20942,7 +20942,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/11th-Movie-Commemoration-Set/Pikachu-Lv10?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G196" s="1">
-        <v>25.66</v>
+        <v>25.64</v>
       </c>
     </row>
     <row r="197">
@@ -21172,7 +21172,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/10th-Movie-Commemoration-Set/Timeless-Celebi?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G206" s="1">
-        <v>14.74</v>
+        <v>14.72</v>
       </c>
     </row>
     <row r="207">
@@ -21195,7 +21195,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/10th-Movie-Commemoration-Set/Wave-Guiding-Hero-Lucario?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G207" s="1">
-        <v>11.44</v>
+        <v>11.43</v>
       </c>
     </row>
     <row r="208">
@@ -21586,7 +21586,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Bonds-to-the-End-of-Time/Flygon-Lv65-Pt2072?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G224" s="1">
-        <v>6.32</v>
+        <v>6.99</v>
       </c>
     </row>
     <row r="225">
@@ -21655,7 +21655,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Bonds-to-the-End-of-Time/Arcanine-Lv53-Pt2010?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=3&amp;isReverseHolo=N</v>
       </c>
       <c r="G227" s="1">
-        <v>10.25</v>
+        <v>9.25</v>
       </c>
     </row>
     <row r="228">
@@ -21701,7 +21701,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Bastiodon-the-Defender/Magmortar-Lv48-BtD?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=3&amp;isReverseHolo=N</v>
       </c>
       <c r="G229" s="1">
-        <v>3.97</v>
+        <v>3.95</v>
       </c>
     </row>
     <row r="230">
@@ -21770,7 +21770,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Space-Time-Creation/Lucario-Lv30-DP1?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=3&amp;isReverseHolo=N</v>
       </c>
       <c r="G232" s="1">
-        <v>3.49</v>
+        <v>3.32</v>
       </c>
     </row>
     <row r="233">
@@ -21793,7 +21793,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Space-Time-Creation/Roserade-Lv33-DP1?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G233" s="1">
-        <v>1</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="234">
@@ -21816,7 +21816,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Shining-Darkness/Gastrodon-East-Sea-Lv43-DP3?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G234" s="1">
-        <v>3.72</v>
+        <v>3.71</v>
       </c>
     </row>
     <row r="235">
@@ -21839,7 +21839,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Intense-Fight-in-the-Destroyed-Sky/Lumineon-Lv38-IFDS020?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G235" s="1">
-        <v>6.8</v>
+        <v>6.63</v>
       </c>
     </row>
     <row r="236">
@@ -21908,7 +21908,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Psycho-Drive/Shaymin-EX-V1?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G238" s="1">
-        <v>4.28</v>
+        <v>4.05</v>
       </c>
     </row>
     <row r="239">
@@ -21977,7 +21977,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Giratina-DPt-Half-Deck/Giratina-Lv70-DPtG008?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G241" s="1">
-        <v>19.99</v>
+        <v>29.97</v>
       </c>
     </row>
     <row r="242">
@@ -22161,7 +22161,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Metagross-Expert-Deck/Jirachi-MED006?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=3&amp;isReverseHolo=N</v>
       </c>
       <c r="G249" s="1">
-        <v>15.38</v>
+        <v>7.2</v>
       </c>
     </row>
     <row r="250">
@@ -22184,7 +22184,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Temple-of-Anger/Mamoswine-Lv54-DP5t?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G250" s="1">
-        <v>3.99</v>
+        <v>4.16</v>
       </c>
     </row>
     <row r="251">
@@ -22253,7 +22253,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Beat-of-the-Frontier/Swampert-Lv60-Pt3029?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G253" s="1">
-        <v>5.21</v>
+        <v>5.48</v>
       </c>
     </row>
     <row r="254">
@@ -22322,7 +22322,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Bonds-to-the-End-of-Time/Bastiodon-GL-Lv41-Pt2067?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G256" s="1">
-        <v>3.81</v>
+        <v>3.98</v>
       </c>
     </row>
     <row r="257">
@@ -22368,7 +22368,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Bonds-to-the-End-of-Time/Mismagius-GL-Lv26-Pt2046?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G258" s="1">
-        <v>6.8</v>
+        <v>8.12</v>
       </c>
     </row>
     <row r="259">
@@ -22414,7 +22414,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Bonds-to-the-End-of-Time/Rampardos-GL-Lv63-Pt2051?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G260" s="1">
-        <v>2.58</v>
+        <v>2.92</v>
       </c>
     </row>
     <row r="261">
@@ -22460,7 +22460,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Secret-of-the-Lakes/Mesprit-Lv50-DP2?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G262" s="1">
-        <v>7.48</v>
+        <v>39.15</v>
       </c>
     </row>
     <row r="263">
@@ -22506,7 +22506,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Secret-of-the-Lakes/Alakazam-Lv47-DP2?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G264" s="1">
-        <v>11.8</v>
+        <v>11.78</v>
       </c>
     </row>
     <row r="265">
@@ -22598,7 +22598,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Space-Time-Creation/Luxray-Lv48-DP1?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G268" s="1">
-        <v>4.86</v>
+        <v>6.18</v>
       </c>
     </row>
     <row r="269">
@@ -22621,7 +22621,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Space-Time-Creation/Roserade-Lv33-DP1?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G269" s="1">
-        <v>1</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="270">
@@ -22667,7 +22667,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Space-Time-Creation/Dusknoir-Lv42-DP1?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G271" s="1">
-        <v>4.96</v>
+        <v>4.13</v>
       </c>
     </row>
     <row r="272">
@@ -22690,7 +22690,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Space-Time-Creation/Shiftry-Lv48-DP1?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G272" s="1">
-        <v>3.48</v>
+        <v>3.32</v>
       </c>
     </row>
     <row r="273">
@@ -22713,7 +22713,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Arceus-LVX-Deck-Lightning-Psychic/Arceus-Lv100-ALP008?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=3&amp;isReverseHolo=N</v>
       </c>
       <c r="G273" s="1">
-        <v>7.41</v>
+        <v>7.4</v>
       </c>
     </row>
     <row r="274">
@@ -22736,7 +22736,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Arceus-LVX-Deck-Lightning-Psychic/Arceus-Lv100-ALP008?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=3&amp;isReverseHolo=N</v>
       </c>
       <c r="G274" s="1">
-        <v>7.41</v>
+        <v>7.4</v>
       </c>
     </row>
     <row r="275">
@@ -22989,7 +22989,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/DPt-Promos/Arceus-Lv100-DPt-P041?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=3&amp;isReverseHolo=N</v>
       </c>
       <c r="G285" s="1">
-        <v>1.97</v>
+        <v>1.95</v>
       </c>
     </row>
     <row r="286">
@@ -23104,7 +23104,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/DP-Promos/Palkia-LVX-DP-P105?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=3&amp;isReverseHolo=N</v>
       </c>
       <c r="G290" s="1">
-        <v>43.82</v>
+        <v>32.48</v>
       </c>
     </row>
     <row r="291">
@@ -23196,7 +23196,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Bonds-to-the-End-of-Time/Alakazam-4-LVX-Pt2042?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G294" s="1">
-        <v>42.66</v>
+        <v>40.99</v>
       </c>
     </row>
     <row r="295">
@@ -23334,7 +23334,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Intense-Fight-in-the-Destroyed-Sky/Giratina-Lv59-IFDS048?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=3&amp;isReverseHolo=N</v>
       </c>
       <c r="G300" s="1">
-        <v>8.4</v>
+        <v>8.39</v>
       </c>
     </row>
     <row r="301">
@@ -23357,7 +23357,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Galactics-Conquest/Giratina-Lv63-Pt1051?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=3&amp;isReverseHolo=N</v>
       </c>
       <c r="G301" s="1">
-        <v>25.85</v>
+        <v>25.82</v>
       </c>
     </row>
     <row r="302">
@@ -23426,7 +23426,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Intense-Fight-in-the-Destroyed-Sky/Regigigas-Lv47-IFDS079?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G304" s="1">
-        <v>5.61</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="305">
@@ -23541,7 +23541,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Intense-Fight-in-the-Destroyed-Sky/Giratina-Lv59-IFDS048?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=3&amp;isReverseHolo=N</v>
       </c>
       <c r="G309" s="1">
-        <v>8.4</v>
+        <v>8.39</v>
       </c>
     </row>
     <row r="310">
@@ -23679,7 +23679,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Terastal-Festival-ex/Sandy-Shocks-ex-V2-sv8a215?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G315" s="1">
-        <v>3.98</v>
+        <v>4.25</v>
       </c>
     </row>
     <row r="316">
@@ -23702,7 +23702,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Terastal-Festival-ex/Zorua-sv8a096?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=Y</v>
       </c>
       <c r="G316" s="1">
-        <v>3.76</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="317">
@@ -24047,7 +24047,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Cry-from-the-Mysterious/Mesprit-LVX-DP5c?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G331" s="1">
-        <v>27.55</v>
+        <v>27.52</v>
       </c>
     </row>
     <row r="332">
@@ -24162,7 +24162,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Moonlit-Pursuit/Cresselia-Lv48-DP4m?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=4&amp;isReverseHolo=N</v>
       </c>
       <c r="G336" s="1">
-        <v>3.45</v>
+        <v>3.38</v>
       </c>
     </row>
     <row r="337">
@@ -24208,7 +24208,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Bonds-to-the-End-of-Time/Mismagius-GL-Lv26-Pt2046?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G338" s="1">
-        <v>6.8</v>
+        <v>8.12</v>
       </c>
     </row>
     <row r="339">
@@ -24277,7 +24277,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Bonds-to-the-End-of-Time/Rampardos-GL-Lv63-Pt2051?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=2&amp;isReverseHolo=N</v>
       </c>
       <c r="G341" s="1">
-        <v>2.58</v>
+        <v>2.92</v>
       </c>
     </row>
     <row r="342">
@@ -24392,7 +24392,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/HeartGold-Collection/Fighting-Energy-L1HG?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=3&amp;isReverseHolo=N</v>
       </c>
       <c r="G346" s="1">
-        <v>19.5</v>
+        <v>14.99</v>
       </c>
     </row>
     <row r="347">
@@ -24415,7 +24415,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/HeartGold-Collection/Fighting-Energy-L1HG?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=3&amp;isReverseHolo=N</v>
       </c>
       <c r="G347" s="1">
-        <v>19.5</v>
+        <v>14.99</v>
       </c>
     </row>
     <row r="348">
@@ -24461,7 +24461,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/HeartGold-Collection/Fire-Energy-L1HG?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=3&amp;isReverseHolo=N</v>
       </c>
       <c r="G349" s="1">
-        <v>8.1</v>
+        <v>8.21</v>
       </c>
     </row>
     <row r="350">
@@ -24576,7 +24576,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Shining-Darkness/Palkia-LVX-DP3?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=3&amp;isReverseHolo=N</v>
       </c>
       <c r="G354" s="1">
-        <v>30.67</v>
+        <v>27.5</v>
       </c>
     </row>
     <row r="355">
@@ -24852,7 +24852,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Arceus-LVX-Deck-Lightning-Psychic/Arceus-Lv100-ALP008?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=3&amp;isReverseHolo=N</v>
       </c>
       <c r="G366" s="1">
-        <v>7.41</v>
+        <v>7.4</v>
       </c>
     </row>
     <row r="367">
@@ -24921,7 +24921,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Arceus-LVX-Deck-Grass-Fire/Arceus-Lv100-AGF005?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=3&amp;isReverseHolo=N</v>
       </c>
       <c r="G369" s="1">
-        <v>7.46</v>
+        <v>6.81</v>
       </c>
     </row>
     <row r="370">
@@ -25013,7 +25013,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Arceus-LVX-Deck-Lightning-Psychic/Arceus-Lv100-ALP003?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=3&amp;isReverseHolo=N</v>
       </c>
       <c r="G373" s="1">
-        <v>5.5</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="374">
@@ -25059,7 +25059,7 @@
         <v>https://www.cardmarket.com/fr/Pokemon/Products/Singles/Arceus-LVX-Deck-Lightning-Psychic/Arceus-Lv100-ALP003?isSigned=N&amp;isPlayset=N&amp;isAltered=N&amp;language=7&amp;minCondition=3&amp;isReverseHolo=N</v>
       </c>
       <c r="G375" s="1">
-        <v>5.5</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="376">

</xml_diff>